<commit_message>
Fine root dynamics in granier model made equal to Sperry
</commit_message>
<xml_diff>
--- a/data-raw/SpParamsDefinition.xlsx
+++ b/data-raw/SpParamsDefinition.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="281">
   <si>
     <t xml:space="preserve">ParameterName</t>
   </si>
@@ -439,6 +439,12 @@
       </rPr>
       <t xml:space="preserve">-2</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Ar2Al</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root area to leaf area ratio</t>
   </si>
   <si>
     <t xml:space="preserve">LeafWidth</t>
@@ -1507,11 +1513,11 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E101" activeCellId="0" sqref="E101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.26"/>
@@ -2374,7 +2380,7 @@
         <v>38</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>39</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2391,58 +2397,58 @@
         <v>38</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>130</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C58" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="D59" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C60" s="0" t="s">
+      <c r="D60" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2450,7 +2456,7 @@
         <v>140</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>141</v>
@@ -2459,24 +2465,24 @@
         <v>38</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C62" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C62" s="0" t="s">
+      <c r="D62" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2490,7 @@
         <v>145</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>146</v>
@@ -2493,7 +2499,7 @@
         <v>38</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2501,7 +2507,7 @@
         <v>147</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>148</v>
@@ -2510,7 +2516,7 @@
         <v>38</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,7 +2524,7 @@
         <v>149</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>150</v>
@@ -2527,7 +2533,7 @@
         <v>38</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2535,7 +2541,7 @@
         <v>151</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>152</v>
@@ -2544,7 +2550,7 @@
         <v>38</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2552,84 +2558,84 @@
         <v>153</v>
       </c>
       <c r="B67" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C67" s="0" t="s">
-        <v>155</v>
-      </c>
       <c r="D67" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C68" s="0" t="s">
+      <c r="D68" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E68" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C69" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C69" s="0" t="s">
+      <c r="D69" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E69" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D69" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B70" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C70" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="C70" s="0" t="s">
-        <v>164</v>
-      </c>
       <c r="D70" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C71" s="0" t="s">
+      <c r="D71" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2637,7 +2643,7 @@
         <v>168</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>169</v>
@@ -2646,7 +2652,7 @@
         <v>38</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2654,7 +2660,7 @@
         <v>170</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>171</v>
@@ -2663,30 +2669,32 @@
         <v>38</v>
       </c>
       <c r="E73" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="s">
+      <c r="B74" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C74" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="D74" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E74" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C74" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E74" s="4"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>177</v>
@@ -2701,7 +2709,7 @@
         <v>178</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C76" s="0" t="s">
         <v>179</v>
@@ -2709,16 +2717,14 @@
       <c r="D76" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E76" s="4" t="s">
-        <v>142</v>
-      </c>
+      <c r="E76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C77" s="0" t="s">
         <v>181</v>
@@ -2727,15 +2733,15 @@
         <v>38</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C78" s="0" t="s">
         <v>183</v>
@@ -2744,30 +2750,32 @@
         <v>38</v>
       </c>
       <c r="E78" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="2" t="s">
+      <c r="B79" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C79" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C79" s="0" t="s">
+      <c r="D79" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E79" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D79" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>188</v>
@@ -2775,16 +2783,14 @@
       <c r="D80" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E80" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C81" s="0" t="s">
         <v>190</v>
@@ -2793,24 +2799,24 @@
         <v>38</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>191</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C82" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C82" s="0" t="s">
+      <c r="D82" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E82" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2818,7 +2824,7 @@
         <v>194</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C83" s="0" t="s">
         <v>195</v>
@@ -2827,21 +2833,24 @@
         <v>38</v>
       </c>
       <c r="E83" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="s">
+      <c r="B84" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C84" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="B84" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C84" s="0" t="s">
+      <c r="D84" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E84" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2849,7 +2858,7 @@
         <v>199</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C85" s="0" t="s">
         <v>200</v>
@@ -2857,16 +2866,13 @@
       <c r="D85" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E85" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
         <v>201</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C86" s="0" t="s">
         <v>202</v>
@@ -2874,22 +2880,25 @@
       <c r="D86" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E86" s="4" t="s">
+      <c r="E86" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="2" t="s">
+      <c r="B87" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C87" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="B87" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C87" s="0" t="s">
+      <c r="D87" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E87" s="4" t="s">
         <v>205</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2897,7 +2906,7 @@
         <v>206</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>207</v>
@@ -2905,16 +2914,13 @@
       <c r="D88" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E88" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
         <v>208</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>209</v>
@@ -2922,22 +2928,25 @@
       <c r="D89" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E89" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E89" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
         <v>210</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C90" s="0" t="s">
         <v>211</v>
       </c>
       <c r="D90" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2945,7 +2954,7 @@
         <v>212</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>213</v>
@@ -2953,16 +2962,13 @@
       <c r="D91" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E91" s="0" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>215</v>
@@ -2970,93 +2976,93 @@
       <c r="D92" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E92" s="4" t="s">
+      <c r="E92" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="5" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="2" t="s">
+      <c r="B93" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="B93" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C93" s="0" t="s">
+      <c r="D93" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E93" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D93" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E93" s="6" t="s">
+    </row>
+    <row r="94" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
+      <c r="B94" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C94" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="B94" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C94" s="0" t="s">
+      <c r="D94" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E94" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E94" s="6" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C95" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="D95" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E95" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="C95" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E95" s="0" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C96" s="0" t="s">
+      <c r="D96" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E96" s="0" t="s">
         <v>228</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C97" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C97" s="0" t="s">
+      <c r="D97" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E97" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3064,7 +3070,7 @@
         <v>232</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>233</v>
@@ -3073,7 +3079,7 @@
         <v>38</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3081,7 +3087,7 @@
         <v>234</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>235</v>
@@ -3090,24 +3096,24 @@
         <v>38</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C100" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C100" s="0" t="s">
+      <c r="D100" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E100" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="D100" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E100" s="7" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3115,7 +3121,7 @@
         <v>239</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C101" s="0" t="s">
         <v>240</v>
@@ -3124,7 +3130,7 @@
         <v>38</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,7 +3138,7 @@
         <v>241</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C102" s="0" t="s">
         <v>242</v>
@@ -3141,100 +3147,100 @@
         <v>38</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C103" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C103" s="0" t="s">
+      <c r="D103" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E103" s="7" t="s">
         <v>245</v>
-      </c>
-      <c r="D103" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E103" s="0" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C104" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C104" s="0" t="s">
+      <c r="D104" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E104" s="0" t="s">
         <v>248</v>
-      </c>
-      <c r="D104" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E104" s="0" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C105" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C105" s="0" t="s">
+      <c r="D105" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E105" s="0" t="s">
         <v>251</v>
-      </c>
-      <c r="D105" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E105" s="0" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C106" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C106" s="0" t="s">
+      <c r="D106" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E106" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="D106" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E106" s="0" t="s">
-        <v>252</v>
-      </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="7" t="s">
+      <c r="A107" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B107" s="7" t="s">
+      <c r="B107" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C107" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="C107" s="0" t="s">
-        <v>257</v>
-      </c>
       <c r="D107" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>39</v>
+        <v>254</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B108" s="7" t="s">
         <v>258</v>
-      </c>
-      <c r="B108" s="7" t="s">
-        <v>256</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>259</v>
@@ -3247,11 +3253,11 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="A109" s="7" t="s">
         <v>260</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C109" s="0" t="s">
         <v>261</v>
@@ -3268,7 +3274,7 @@
         <v>262</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C110" s="0" t="s">
         <v>263</v>
@@ -3285,7 +3291,7 @@
         <v>264</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C111" s="0" t="s">
         <v>265</v>
@@ -3294,24 +3300,24 @@
         <v>38</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>266</v>
+        <v>39</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C112" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="B112" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="C112" s="0" t="s">
+      <c r="D112" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E112" s="0" t="s">
         <v>268</v>
-      </c>
-      <c r="D112" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E112" s="0" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3319,7 +3325,7 @@
         <v>269</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C113" s="0" t="s">
         <v>270</v>
@@ -3328,7 +3334,7 @@
         <v>38</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3336,7 +3342,7 @@
         <v>271</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>272</v>
@@ -3353,7 +3359,7 @@
         <v>273</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>274</v>
@@ -3362,7 +3368,7 @@
         <v>38</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,7 +3376,7 @@
         <v>275</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>276</v>
@@ -3379,7 +3385,7 @@
         <v>38</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>165</v>
+        <v>89</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3387,7 +3393,7 @@
         <v>277</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>278</v>
@@ -3396,10 +3402,26 @@
         <v>38</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
RER based on N
</commit_message>
<xml_diff>
--- a/data-raw/SpParamsDefinition.xlsx
+++ b/data-raw/SpParamsDefinition.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="285">
   <si>
     <t xml:space="preserve">ParameterName</t>
   </si>
@@ -980,21 +980,52 @@
     <t xml:space="preserve">Parameter d of the root xylem vulnerability curve</t>
   </si>
   <si>
-    <t xml:space="preserve">Narea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrogen mass per leaf area</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">g N·m</t>
+    <t xml:space="preserve">Vmax298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Rubisco carboxilation rate</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t xml:space="preserve">m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">mol CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·s</t>
     </r>
     <r>
       <rPr>
@@ -1005,14 +1036,35 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">-2</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Vmax298</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum Rubisco carboxilation rate</t>
+    <t xml:space="preserve">Jmax298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum rate of electron transport at 298K</t>
   </si>
   <si>
     <r>
@@ -1033,28 +1085,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">mol CO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">·s</t>
+      <t xml:space="preserve">mol electrons·s</t>
     </r>
     <r>
       <rPr>
@@ -1090,73 +1121,34 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Jmax298</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum rate of electron transport at 298K</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t xml:space="preserve">m</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">mol electrons·s</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">·m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-2</t>
-    </r>
+    <t xml:space="preserve">Nleaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen mass per leaf dry mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mg N / g dry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nsapwood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen mass per sapwood dry mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nfineroot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrogen mass per fine root dry mass</t>
   </si>
   <si>
     <t xml:space="preserve">WoodC</t>
   </si>
   <si>
-    <t xml:space="preserve">Growth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wood carbon content per dry weight </t>
+    <t xml:space="preserve">Wood carbon content per dry mass </t>
   </si>
   <si>
     <t xml:space="preserve">g C / g dry</t>
@@ -1513,11 +1505,11 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C56" activeCellId="0" sqref="C56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A96" activeCellId="0" sqref="A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.26"/>
@@ -2980,8 +2972,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5" t="s">
+    <row r="93" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="s">
         <v>216</v>
       </c>
       <c r="B93" s="5" t="s">
@@ -2993,11 +2985,11 @@
       <c r="D93" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E93" s="4" t="s">
+      <c r="E93" s="6" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
         <v>219</v>
       </c>
@@ -3027,7 +3019,7 @@
       <c r="D95" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E95" s="6" t="s">
+      <c r="E95" s="0" t="s">
         <v>224</v>
       </c>
     </row>
@@ -3045,58 +3037,58 @@
         <v>38</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E97" s="7" t="s">
-        <v>231</v>
+      <c r="E97" s="0" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E98" s="7" t="s">
-        <v>231</v>
+      <c r="E98" s="0" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C99" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E99" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="D99" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3113,41 +3105,41 @@
         <v>38</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C102" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E102" s="7" t="s">
         <v>242</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E102" s="7" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,117 +3156,117 @@
         <v>38</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E104" s="0" t="s">
-        <v>248</v>
+      <c r="E104" s="7" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D105" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E105" s="0" t="s">
-        <v>251</v>
+      <c r="E105" s="7" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E106" s="0" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>226</v>
       </c>
       <c r="C107" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D107" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E107" s="0" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="7" t="s">
+      <c r="B108" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C108" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="B108" s="7" t="s">
+      <c r="D108" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E108" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="C108" s="0" t="s">
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D108" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E108" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="7" t="s">
+      <c r="B109" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C109" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="D109" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E109" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="C109" s="0" t="s">
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="D109" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E109" s="0" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="B110" s="7" t="s">
         <v>262</v>
-      </c>
-      <c r="B110" s="7" t="s">
-        <v>258</v>
       </c>
       <c r="C110" s="0" t="s">
         <v>263</v>
@@ -3287,11 +3279,11 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="A111" s="7" t="s">
         <v>264</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C111" s="0" t="s">
         <v>265</v>
@@ -3308,7 +3300,7 @@
         <v>266</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>267</v>
@@ -3317,41 +3309,41 @@
         <v>38</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>268</v>
+        <v>39</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C113" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="B113" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="C113" s="0" t="s">
-        <v>270</v>
-      </c>
       <c r="D113" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C114" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="B114" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="C114" s="0" t="s">
+      <c r="D114" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E114" s="0" t="s">
         <v>272</v>
-      </c>
-      <c r="D114" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E114" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3359,7 +3351,7 @@
         <v>273</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C115" s="0" t="s">
         <v>274</v>
@@ -3368,7 +3360,7 @@
         <v>38</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3376,7 +3368,7 @@
         <v>275</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C116" s="0" t="s">
         <v>276</v>
@@ -3385,7 +3377,7 @@
         <v>38</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3393,7 +3385,7 @@
         <v>277</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>278</v>
@@ -3402,7 +3394,7 @@
         <v>38</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>167</v>
+        <v>44</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3410,7 +3402,7 @@
         <v>279</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C118" s="0" t="s">
         <v>280</v>
@@ -3419,11 +3411,43 @@
         <v>38</v>
       </c>
       <c r="E118" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E120" s="0" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
new parameters for dispersal
</commit_message>
<xml_diff>
--- a/data-raw/SpParamsDefinition.xlsx
+++ b/data-raw/SpParamsDefinition.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="331">
   <si>
     <t xml:space="preserve">ParameterName</t>
   </si>
@@ -1281,6 +1281,9 @@
     <t xml:space="preserve">Seed dry mass</t>
   </si>
   <si>
+    <t xml:space="preserve">mg</t>
+  </si>
+  <si>
     <t xml:space="preserve">SeedLongevity</t>
   </si>
   <si>
@@ -1288,6 +1291,21 @@
   </si>
   <si>
     <t xml:space="preserve">yr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DispersalDistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance parameter for dispersal kernel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DispersalShape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shape parameter for dispersal kernel</t>
   </si>
   <si>
     <t xml:space="preserve">ProbRecr</t>
@@ -1574,13 +1592,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E120" activeCellId="0" sqref="E120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.26"/>
@@ -3519,137 +3537,134 @@
         <v>38</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>176</v>
+        <v>289</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="6" t="s">
-        <v>292</v>
+      <c r="A122" s="0" t="s">
+        <v>293</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D122" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>63</v>
+        <v>295</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D123" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E123" s="0" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
-        <v>296</v>
+      <c r="A124" s="6" t="s">
+        <v>298</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D124" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>171</v>
+        <v>63</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D125" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E125" s="0" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="6" t="s">
-        <v>300</v>
+      <c r="A126" s="0" t="s">
+        <v>302</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E126" s="0" t="s">
-        <v>39</v>
+        <v>171</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E127" s="0" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
-        <v>304</v>
+      <c r="A128" s="6" t="s">
+        <v>306</v>
       </c>
       <c r="B128" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>38</v>
@@ -3660,115 +3675,115 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B129" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E129" s="0" t="s">
-        <v>308</v>
+        <v>39</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D130" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E130" s="0" t="s">
-        <v>143</v>
+        <v>39</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D131" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E131" s="0" t="s">
-        <v>44</v>
+        <v>314</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D132" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E132" s="0" t="s">
-        <v>44</v>
+        <v>143</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>285</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E133" s="0" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C134" s="6" t="s">
-        <v>318</v>
+      <c r="C134" s="0" t="s">
+        <v>320</v>
       </c>
       <c r="D134" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C135" s="6" t="s">
-        <v>320</v>
+      <c r="C135" s="0" t="s">
+        <v>322</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>38</v>
@@ -3779,40 +3794,72 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C136" s="0" t="s">
-        <v>322</v>
+      <c r="C136" s="6" t="s">
+        <v>324</v>
       </c>
       <c r="D136" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C137" s="0" t="s">
-        <v>324</v>
+      <c r="C137" s="6" t="s">
+        <v>326</v>
       </c>
       <c r="D137" s="0" t="s">
         <v>38</v>
       </c>
       <c r="E137" s="0" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="D138" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E138" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="C139" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D139" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E139" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
beta distribution for leaf angles
</commit_message>
<xml_diff>
--- a/data-raw/SpParamsDefinition.xlsx
+++ b/data-raw/SpParamsDefinition.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="363">
   <si>
     <t xml:space="preserve">ParameterName</t>
   </si>
@@ -548,6 +548,18 @@
   </si>
   <si>
     <t xml:space="preserve">degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LeafAngleSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation of the leaf angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClumpingIndex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canopy clumping index</t>
   </si>
   <si>
     <t xml:space="preserve">gammaSWR</t>
@@ -1680,10 +1692,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C78" activeCellId="0" sqref="C78"/>
+      <selection pane="topLeft" activeCell="D77" activeCellId="0" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2898,41 +2910,41 @@
         <v>42</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>173</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>173</v>
       </c>
       <c r="C78" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2949,45 +2961,49 @@
         <v>42</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>188</v>
-      </c>
       <c r="D80" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E80" s="4"/>
+      <c r="E80" s="4" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E81" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C81" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E81" s="4"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>191</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>187</v>
       </c>
       <c r="C82" s="0" t="s">
         <v>192</v>
@@ -2995,78 +3011,78 @@
       <c r="D82" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E82" s="4" t="s">
-        <v>193</v>
-      </c>
+      <c r="E82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C83" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C83" s="0" t="s">
+      <c r="D83" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D83" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E83" s="4"/>
-    </row>
-    <row r="84" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="2" t="s">
+      <c r="B84" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C84" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="B84" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C84" s="0" t="s">
+      <c r="D84" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E84" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C85" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B85" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C85" s="0" t="s">
+      <c r="D85" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D85" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E85" s="4"/>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="2" t="s">
+      <c r="B86" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C86" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="B86" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C86" s="0" t="s">
+      <c r="D86" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E86" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D86" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C87" s="0" t="s">
         <v>204</v>
@@ -3081,58 +3097,54 @@
         <v>205</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C88" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C88" s="0" t="s">
         <v>206</v>
       </c>
       <c r="D88" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E88" s="4" t="s">
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="89" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="2" t="s">
+      <c r="B89" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C89" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="B89" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>209</v>
-      </c>
       <c r="D89" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E89" s="4" t="s">
-        <v>207</v>
-      </c>
+      <c r="E89" s="4"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B90" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C90" s="0" t="s">
+      <c r="D90" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E90" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D90" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="91" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C91" s="0" t="s">
         <v>213</v>
@@ -3140,14 +3152,16 @@
       <c r="D91" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E91" s="4"/>
+      <c r="E91" s="4" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
         <v>214</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C92" s="0" t="s">
         <v>215</v>
@@ -3156,7 +3170,7 @@
         <v>42</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>193</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,7 +3178,7 @@
         <v>216</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>217</v>
@@ -3172,59 +3186,57 @@
       <c r="D93" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E93" s="4" t="s">
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="2" t="s">
+      <c r="B94" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C94" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B94" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>220</v>
-      </c>
       <c r="D94" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E95" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B95" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C95" s="0" t="s">
+    </row>
+    <row r="96" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D95" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="2" t="s">
+      <c r="B96" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C96" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="B96" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C96" s="0" t="s">
+      <c r="D96" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E96" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E96" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,7 +3244,7 @@
         <v>226</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>227</v>
@@ -3241,7 +3253,7 @@
         <v>42</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3249,7 +3261,7 @@
         <v>228</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>229</v>
@@ -3258,15 +3270,15 @@
         <v>42</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
         <v>230</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>231</v>
@@ -3275,41 +3287,41 @@
         <v>42</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C100" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C100" s="0" t="s">
+      <c r="D100" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D100" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E100" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2" t="s">
+      <c r="B101" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C101" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="B101" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C101" s="0" t="s">
+      <c r="D101" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E101" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3317,7 +3329,7 @@
         <v>237</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C102" s="0" t="s">
         <v>238</v>
@@ -3326,7 +3338,7 @@
         <v>42</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3334,7 +3346,7 @@
         <v>239</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C103" s="0" t="s">
         <v>240</v>
@@ -3343,15 +3355,15 @@
         <v>42</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
         <v>241</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C104" s="0" t="s">
         <v>242</v>
@@ -3360,7 +3372,7 @@
         <v>42</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3368,7 +3380,7 @@
         <v>243</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C105" s="0" t="s">
         <v>244</v>
@@ -3377,15 +3389,15 @@
         <v>42</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
         <v>245</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C106" s="0" t="s">
         <v>246</v>
@@ -3394,7 +3406,7 @@
         <v>42</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>193</v>
+        <v>236</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,7 +3414,7 @@
         <v>247</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C107" s="0" t="s">
         <v>248</v>
@@ -3411,7 +3423,7 @@
         <v>42</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3419,7 +3431,7 @@
         <v>249</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>250</v>
@@ -3428,15 +3440,15 @@
         <v>42</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
         <v>251</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C109" s="0" t="s">
         <v>252</v>
@@ -3444,84 +3456,84 @@
       <c r="D109" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E109" s="8" t="s">
-        <v>253</v>
+      <c r="E109" s="4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C110" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C110" s="0" t="s">
+      <c r="D110" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D110" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E110" s="8" t="s">
+      <c r="B111" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C111" s="0" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="2" t="s">
+      <c r="D111" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E111" s="8" t="s">
         <v>257</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C111" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="D111" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E111" s="0" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E112" s="8" t="s">
         <v>260</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C112" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="D112" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E112" s="0" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E113" s="0" t="s">
         <v>263</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C113" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="D113" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E113" s="0" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="C114" s="0" t="s">
         <v>266</v>
@@ -3530,58 +3542,58 @@
         <v>42</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C115" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C115" s="0" t="s">
-        <v>269</v>
-      </c>
       <c r="D115" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E115" s="6" t="s">
-        <v>270</v>
+      <c r="E115" s="0" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E116" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C116" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="D116" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E116" s="6" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C117" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C117" s="0" t="s">
+      <c r="D117" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="D117" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3589,7 +3601,7 @@
         <v>275</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C118" s="0" t="s">
         <v>276</v>
@@ -3598,41 +3610,41 @@
         <v>42</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C119" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>279</v>
-      </c>
       <c r="D119" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C120" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C120" s="0" t="s">
+      <c r="D120" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E120" s="6" t="s">
         <v>281</v>
-      </c>
-      <c r="D120" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E120" s="6" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3640,7 +3652,7 @@
         <v>282</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C121" s="0" t="s">
         <v>283</v>
@@ -3649,109 +3661,109 @@
         <v>42</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C122" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C122" s="0" t="s">
-        <v>286</v>
-      </c>
       <c r="D122" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E122" s="0" t="s">
-        <v>287</v>
+      <c r="E122" s="6" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E123" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C123" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="D123" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E123" s="0" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E124" s="0" t="s">
         <v>291</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C124" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="D124" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E124" s="0" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E125" s="0" t="s">
         <v>294</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C125" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="D125" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E125" s="0" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="D126" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E126" s="0" t="s">
         <v>297</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C126" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="D126" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E126" s="0" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C127" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C127" s="0" t="s">
+      <c r="D127" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E127" s="0" t="s">
         <v>300</v>
-      </c>
-      <c r="D127" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E127" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3759,160 +3771,163 @@
         <v>301</v>
       </c>
       <c r="B128" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C128" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="C128" s="0" t="s">
-        <v>303</v>
-      </c>
       <c r="D128" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>302</v>
+        <v>265</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E129" s="0" t="s">
-        <v>307</v>
+        <v>67</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E130" s="0" t="s">
         <v>308</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C130" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="D130" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C131" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="C131" s="0" t="s">
+      <c r="D131" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E131" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="D131" s="0" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="6" t="s">
+      <c r="A132" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B132" s="6" t="s">
+      <c r="B132" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C132" s="0" t="s">
         <v>313</v>
       </c>
-      <c r="C132" s="0" t="s">
+      <c r="D132" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D132" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E132" s="0" t="s">
+      <c r="B133" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="D134" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E134" s="0" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="B133" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C133" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="D133" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E133" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="B134" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C134" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="D134" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E134" s="0" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="D135" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E135" s="0" t="s">
         <v>321</v>
-      </c>
-      <c r="B135" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C135" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="D135" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E135" s="0" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="D136" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E136" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="B136" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C136" s="0" t="s">
+    </row>
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="D136" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="6" t="s">
+      <c r="B137" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C137" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="B137" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C137" s="0" t="s">
+      <c r="D137" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E137" s="0" t="s">
         <v>327</v>
-      </c>
-      <c r="D137" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E137" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3920,7 +3935,7 @@
         <v>328</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C138" s="0" t="s">
         <v>329</v>
@@ -3928,16 +3943,13 @@
       <c r="D138" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E138" s="0" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+      <c r="A139" s="6" t="s">
         <v>330</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C139" s="0" t="s">
         <v>331</v>
@@ -3946,7 +3958,7 @@
         <v>42</v>
       </c>
       <c r="E139" s="0" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3954,7 +3966,7 @@
         <v>332</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C140" s="0" t="s">
         <v>333</v>
@@ -3963,15 +3975,15 @@
         <v>42</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="0" t="s">
         <v>334</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C141" s="0" t="s">
         <v>335</v>
@@ -3980,7 +3992,7 @@
         <v>42</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>43</v>
+        <v>182</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3988,7 +4000,7 @@
         <v>336</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C142" s="0" t="s">
         <v>337</v>
@@ -3997,15 +4009,15 @@
         <v>42</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
+      <c r="A143" s="6" t="s">
         <v>338</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C143" s="0" t="s">
         <v>339</v>
@@ -4022,7 +4034,7 @@
         <v>340</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C144" s="0" t="s">
         <v>341</v>
@@ -4031,41 +4043,41 @@
         <v>42</v>
       </c>
       <c r="E144" s="0" t="s">
-        <v>342</v>
+        <v>43</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C145" s="0" t="s">
         <v>343</v>
       </c>
-      <c r="B145" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C145" s="0" t="s">
-        <v>344</v>
-      </c>
       <c r="D145" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>147</v>
+        <v>43</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C146" s="0" t="s">
         <v>345</v>
       </c>
-      <c r="B146" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C146" s="0" t="s">
+      <c r="D146" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E146" s="0" t="s">
         <v>346</v>
-      </c>
-      <c r="D146" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E146" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4073,7 +4085,7 @@
         <v>347</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C147" s="0" t="s">
         <v>348</v>
@@ -4082,7 +4094,7 @@
         <v>42</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4090,7 +4102,7 @@
         <v>349</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C148" s="0" t="s">
         <v>350</v>
@@ -4099,7 +4111,7 @@
         <v>42</v>
       </c>
       <c r="E148" s="0" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4107,16 +4119,16 @@
         <v>351</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C149" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C149" s="0" t="s">
         <v>352</v>
       </c>
       <c r="D149" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E149" s="0" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4124,9 +4136,9 @@
         <v>353</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C150" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C150" s="0" t="s">
         <v>354</v>
       </c>
       <c r="D150" s="0" t="s">
@@ -4141,16 +4153,16 @@
         <v>355</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C151" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="C151" s="6" t="s">
         <v>356</v>
       </c>
       <c r="D151" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E151" s="0" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4158,19 +4170,52 @@
         <v>357</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C152" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="C152" s="6" t="s">
         <v>358</v>
       </c>
       <c r="D152" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C153" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="D153" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E153" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B154" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C154" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="D154" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E154" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
accepted name not strict parameter
</commit_message>
<xml_diff>
--- a/data-raw/SpParamsDefinition.xlsx
+++ b/data-raw/SpParamsDefinition.xlsx
@@ -782,6 +782,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">mol H</t>
     </r>
@@ -792,6 +793,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -801,6 +803,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">O * </t>
     </r>
@@ -820,6 +823,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">mol CO</t>
     </r>
@@ -830,6 +834,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -840,6 +845,7 @@
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-1</t>
     </r>
@@ -1589,7 +1595,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* \-??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1654,29 +1660,9 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Symbol"/>
       <family val="1"/>
       <charset val="2"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1734,7 +1720,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1771,10 +1757,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1796,8 +1778,8 @@
   </sheetPr>
   <dimension ref="A1:F155"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A94" activeCellId="0" sqref="A94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1806,7 +1788,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="70.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,7 +1859,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3545,7 +3527,7 @@
       <c r="D92" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E92" s="8" t="s">
+      <c r="E92" s="4" t="s">
         <v>217</v>
       </c>
       <c r="F92" s="0" t="n">
@@ -3943,7 +3925,7 @@
       <c r="D112" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E112" s="9" t="s">
+      <c r="E112" s="8" t="s">
         <v>261</v>
       </c>
       <c r="F112" s="0" t="n">
@@ -3963,7 +3945,7 @@
       <c r="D113" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="E113" s="9" t="s">
+      <c r="E113" s="8" t="s">
         <v>264</v>
       </c>
       <c r="F113" s="0" t="n">

</xml_diff>

<commit_message>
seedlingBank and seedling recruitment
</commit_message>
<xml_diff>
--- a/data-raw/SpParamsDefinition.xlsx
+++ b/data-raw/SpParamsDefinition.xlsx
@@ -1524,10 +1524,10 @@
     <t xml:space="preserve">Minimum percentage of PAR at the ground level for successful recruitment</t>
   </si>
   <si>
-    <t xml:space="preserve">RecrTreeDBH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recruitment tree dbh (typically 1 cm)</t>
+    <t xml:space="preserve">RecrAge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age of recruiment</t>
   </si>
   <si>
     <t xml:space="preserve">RecrTreeHeight</t>
@@ -1900,8 +1900,8 @@
   </sheetPr>
   <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B139" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E149" activeCellId="0" sqref="E149"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C146" activeCellId="0" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4706,23 +4706,20 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="7" t="s">
+      <c r="A146" s="0" t="s">
         <v>346</v>
       </c>
-      <c r="B146" s="7" t="s">
+      <c r="B146" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="C146" s="1" t="s">
+      <c r="C146" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="D146" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F146" s="1" t="n">
-        <v>0</v>
+      <c r="D146" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E146" s="0" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
RecrZ50 and RecrZ95 removed
</commit_message>
<xml_diff>
--- a/data-raw/SpParamsDefinition.xlsx
+++ b/data-raw/SpParamsDefinition.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="367">
   <si>
     <t xml:space="preserve">ParameterName</t>
   </si>
@@ -1555,18 +1555,6 @@
   </si>
   <si>
     <t xml:space="preserve">Recruitment shrub cover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RecrZ50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recruitment depth corresponding to 50% of fine roots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RecrZ95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recruitment depth corresponding to 95% of fine roots</t>
   </si>
   <si>
     <t xml:space="preserve">RespFire</t>
@@ -1898,10 +1886,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C146" activeCellId="0" sqref="C146"/>
+      <selection pane="topLeft" activeCell="C153" activeCellId="0" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4706,19 +4694,19 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+      <c r="A146" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B146" s="0" t="s">
+      <c r="B146" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C146" s="0" t="s">
+      <c r="C146" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D146" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="E146" s="0" t="s">
+      <c r="D146" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E146" s="1" t="s">
         <v>332</v>
       </c>
     </row>
@@ -4816,7 +4804,7 @@
         <v>43</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="F151" s="1" t="n">
         <v>0</v>
@@ -4829,14 +4817,14 @@
       <c r="B152" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="C152" s="1" t="s">
+      <c r="C152" s="7" t="s">
         <v>360</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="F152" s="1" t="n">
         <v>0</v>
@@ -4849,7 +4837,7 @@
       <c r="B153" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="C153" s="1" t="s">
+      <c r="C153" s="7" t="s">
         <v>362</v>
       </c>
       <c r="D153" s="1" t="s">
@@ -4869,14 +4857,14 @@
       <c r="B154" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="C154" s="7" t="s">
+      <c r="C154" s="1" t="s">
         <v>364</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>70</v>
+        <v>354</v>
       </c>
       <c r="F154" s="1" t="n">
         <v>0</v>
@@ -4889,59 +4877,21 @@
       <c r="B155" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="C155" s="7" t="s">
+      <c r="C155" s="1" t="s">
         <v>366</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="F155" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E156" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="F156" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="B157" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D157" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E157" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F157" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>